<commit_message>
docs: Update for test of workflow
</commit_message>
<xml_diff>
--- a/data/books.xlsx
+++ b/data/books.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -127,24 +127,6 @@
   </si>
   <si>
     <t>초록달팽이에서 처음으로 나온 동화책이다. 그동안 동시, 동화, 그림책 등 여러 장르를 넘나들며 독자들에게 많은 관심과 사랑을 받아 온 이묘신 작가가 자신의 경험을 한 편의 따뜻하고 아름다운 이야기로 꾸몄다."</t>
-  </si>
-  <si>
-    <t>f76eb274</t>
-  </si>
-  <si>
-    <t>날아라, 씨앗 폭탄!</t>
-  </si>
-  <si>
-    <t>가로세로그림책</t>
-  </si>
-  <si>
-    <t>초록개구리</t>
-  </si>
-  <si>
-    <t>2024-05-25</t>
-  </si>
-  <si>
-    <t>달달숲 마을엔 나무가 없다. 사람들이 모조리 베어 가서 그루터기만 가득하다. 어느 날, 어른 동물들은 ‘폭탄’을 만들기로 한다. 그 소식을 엿들은 아기 여우는 헐레벌떡 친구들에게 달려간다. 아기 동물들은 어른들이 전쟁을 벌일 거라는 생각에 그 ‘폭탄’을 찾아서 꼭꼭 숨긴다. 그런데… 참 이상해하다. 며칠 뒤 ‘폭탄’을 숨긴 곳에 파릇파릇한 싹이 돋아난 것이다. 이 수상한 폭탄의 정체는 무엇일까?"</t>
   </si>
 </sst>
 </file>
@@ -152,7 +134,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -222,7 +204,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +509,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="16.5"/>
@@ -700,42 +682,11 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="8">
-        <v>17</v>
-      </c>
-      <c r="G5" s="8">
-        <v>44</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
chore: Update Excel for testing
</commit_message>
<xml_diff>
--- a/data/books.xlsx
+++ b/data/books.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Title</t>
   </si>
@@ -127,6 +127,34 @@
   </si>
   <si>
     <t>초록달팽이에서 처음으로 나온 동화책이다. 그동안 동시, 동화, 그림책 등 여러 장르를 넘나들며 독자들에게 많은 관심과 사랑을 받아 온 이묘신 작가가 자신의 경험을 한 편의 따뜻하고 아름다운 이야기로 꾸몄다."</t>
+  </si>
+  <si>
+    <t>f76eb274</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날아라, 씨앗 폭탄!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>가로세로그림책</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초록개구리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024-05-25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9791157822973</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>달달숲 마을엔 나무가 없다. 사람들이 모조리 베어 가서 그루터기만 가득하다. 어느 날, 어른 동물들은 ‘폭탄’을 만들기로 한다. 그 소식을 엿들은 아기 여우는 헐레벌떡 친구들에게 달려간다. 아기 동물들은 어른들이 전쟁을 벌일 거라는 생각에 그 ‘폭탄’을 찾아서 꼭꼭 숨긴다. 그런데… 참 이상해하다. 며칠 뒤 ‘폭탄’을 숨긴 곳에 파릇파릇한 싹이 돋아난 것이다. 이 수상한 폭탄의 정체는 무엇일까?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -509,7 +537,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="16.5"/>
@@ -682,11 +710,42 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="B5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="3"/>
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="8">
+        <v>17</v>
+      </c>
+      <c r="G5" s="8">
+        <v>44</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
chore: Update xlsx file to test
</commit_message>
<xml_diff>
--- a/data/books.xlsx
+++ b/data/books.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Title</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Writer</t>
   </si>
   <si>
-    <t>2024-07-01</t>
-  </si>
-  <si>
     <t>SeriesNumber</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>시인은 아이의 눈과 입을 빌어 아빠에게서 배려와 느림의 철학을, 할머니에게서 따뜻한 마음과 자연의 소중함을, 엄마에게서 위로와 격려를, 이모에게서 긍정적인 사고를 이야기한다.</t>
   </si>
   <si>
-    <t>2024-07-25</t>
-  </si>
-  <si>
     <t>68e75fa3</t>
   </si>
   <si>
@@ -154,6 +148,26 @@
   </si>
   <si>
     <t>달달숲 마을엔 나무가 없다. 사람들이 모조리 베어 가서 그루터기만 가득하다. 어느 날, 어른 동물들은 ‘폭탄’을 만들기로 한다. 그 소식을 엿들은 아기 여우는 헐레벌떡 친구들에게 달려간다. 아기 동물들은 어른들이 전쟁을 벌일 거라는 생각에 그 ‘폭탄’을 찾아서 꼭꼭 숨긴다. 그런데… 참 이상해하다. 며칠 뒤 ‘폭탄’을 숨긴 곳에 파릇파릇한 싹이 돋아난 것이다. 이 수상한 폭탄의 정체는 무엇일까?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ebook</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024-08-01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024-08-25</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -209,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -233,6 +247,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -534,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="16.5"/>
@@ -553,13 +573,15 @@
     <col min="9" max="9" width="18" style="2" customWidth="1"/>
     <col min="10" max="10" width="22.125" style="2" customWidth="1"/>
     <col min="11" max="11" width="16.75" style="2" customWidth="1"/>
-    <col min="12" max="12" width="47.25" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="11.375" style="2"/>
+    <col min="12" max="12" width="9.125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="7.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="47.25" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="11.375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33">
+    <row r="1" spans="1:14" ht="33">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -574,7 +596,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -592,24 +614,30 @@
         <v>7</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="115.5">
+    <row r="2" spans="1:14" ht="115.5">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="8">
         <v>5</v>
@@ -618,36 +646,42 @@
         <v>80</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="66">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="66">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="8">
         <v>9</v>
@@ -656,36 +690,42 @@
         <v>64</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="9">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F4" s="8">
         <v>1</v>
@@ -694,36 +734,42 @@
         <v>76</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="F5" s="8">
         <v>17</v>
@@ -732,19 +778,25 @@
         <v>44</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Update demo data
</commit_message>
<xml_diff>
--- a/data/books.xlsx
+++ b/data/books.xlsx
@@ -151,10 +151,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Ebook</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Type</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -168,6 +164,10 @@
   </si>
   <si>
     <t>2024-08-25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BookFormat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -557,7 +557,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="16.5"/>
@@ -614,10 +614,10 @@
         <v>7</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>8</v>
@@ -628,7 +628,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>23</v>
@@ -672,7 +672,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>27</v>
@@ -716,7 +716,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>34</v>
@@ -760,7 +760,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>36</v>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>41</v>

</xml_diff>